<commit_message>
check token, round configure
</commit_message>
<xml_diff>
--- a/AssociatedApp/2NumKakkKak_DB.xlsx
+++ b/AssociatedApp/2NumKakkKak_DB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpaceGit\WM-LOTTO-APP\AssociatedApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpaceSTS4\Git\BackEnd\WM-LOTTO-APP\AssociatedApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="112">
   <si>
     <t>Table</t>
   </si>
@@ -324,6 +324,42 @@
   </si>
   <si>
     <t>etc value</t>
+  </si>
+  <si>
+    <t>RoundConfigure</t>
+  </si>
+  <si>
+    <t>RCF_ID</t>
+  </si>
+  <si>
+    <t>2019051 (YYYYMMR)</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>R_YEAR</t>
+  </si>
+  <si>
+    <t>2019 …</t>
+  </si>
+  <si>
+    <t>R_MONTH</t>
+  </si>
+  <si>
+    <t>1 to 12</t>
+  </si>
+  <si>
+    <t>R_ROUND</t>
+  </si>
+  <si>
+    <t>1 …</t>
+  </si>
+  <si>
+    <t>R_STATUS</t>
+  </si>
+  <si>
+    <t>ACTIVE / DISABLE</t>
   </si>
 </sst>
 </file>
@@ -365,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -374,6 +410,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G132"/>
+  <dimension ref="A2:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2500,7 +2543,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>15</v>
       </c>
@@ -2511,7 +2554,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>65</v>
       </c>
@@ -2525,7 +2568,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>13</v>
       </c>
@@ -2536,7 +2579,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>66</v>
       </c>
@@ -2547,6 +2590,194 @@
         <v>255</v>
       </c>
       <c r="F132" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="4"/>
+      <c r="B134" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D134" s="4"/>
+      <c r="E134" s="4"/>
+      <c r="F134" s="4"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="4"/>
+      <c r="B135" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E135" s="4"/>
+      <c r="F135" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D136" s="4">
+        <v>255</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F136" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D137" s="4">
+        <v>0</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D138" s="4">
+        <v>0</v>
+      </c>
+      <c r="E138" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D139" s="4">
+        <v>0</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F139" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D140" s="4">
+        <v>255</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="4"/>
+      <c r="B141" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D141" s="4"/>
+      <c r="E141" s="4"/>
+      <c r="F141" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="4"/>
+      <c r="B142" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D142" s="4">
+        <v>255</v>
+      </c>
+      <c r="E142" s="4"/>
+      <c r="F142" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" s="4"/>
+      <c r="B143" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D143" s="4"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="4"/>
+      <c r="B144" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D144" s="4">
+        <v>255</v>
+      </c>
+      <c r="E144" s="4"/>
+      <c r="F144" s="5" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>